<commit_message>
Anda todo con el precio_2 , pero quedo todo desordenado. Hay que sacar los radius de nuevo, acomodar estetica general, poner alert cuando se esta quedando sin insumos, etc
</commit_message>
<xml_diff>
--- a/reporte_clientes_2025-02-25_a_2025-02-27.xlsx
+++ b/reporte_clientes_2025-02-25_a_2025-02-27.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,25 +488,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>237000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gonzalo</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>113819138</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>142200</v>
+        <v>94800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>